<commit_message>
make the SES column names more robust; start implementing analyses and plots in metasem. Think about some multiplot output (move this to cowplot)
</commit_message>
<xml_diff>
--- a/inst/extdata/GxSES/data_GxSES.xlsx
+++ b/inst/extdata/GxSES/data_GxSES.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="0" windowWidth="24860" windowHeight="14720" tabRatio="547" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -37,39 +37,18 @@
     <t>a</t>
   </si>
   <si>
-    <t xml:space="preserve">a SE </t>
-  </si>
-  <si>
-    <t>a'</t>
-  </si>
-  <si>
-    <t>a' SE</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
-    <t>c' SE</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
     <t>e SE</t>
   </si>
   <si>
-    <t>e'</t>
-  </si>
-  <si>
-    <t>e' SE</t>
-  </si>
-  <si>
     <t>c SE</t>
   </si>
   <si>
-    <t>c'</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -175,9 +154,6 @@
     <t>g</t>
   </si>
   <si>
-    <t>Age (Yrs)</t>
-  </si>
-  <si>
     <t>Jacobson [Rowe, Jacobson, &amp; Van den Oord (1999)]</t>
   </si>
   <si>
@@ -262,9 +238,6 @@
     <t>CoSMoS</t>
   </si>
   <si>
-    <t>N (Pairs)</t>
-  </si>
-  <si>
     <t>Netherlands Twin Registry (Child)</t>
   </si>
   <si>
@@ -313,39 +286,18 @@
     <t>a_z</t>
   </si>
   <si>
-    <t>a SE _z</t>
-  </si>
-  <si>
-    <t>a'_z</t>
-  </si>
-  <si>
-    <t>a' SE_z</t>
-  </si>
-  <si>
     <t>c_z</t>
   </si>
   <si>
     <t>c SE_z</t>
   </si>
   <si>
-    <t>c'_z</t>
-  </si>
-  <si>
-    <t>c' SE_z</t>
-  </si>
-  <si>
     <t>e_z</t>
   </si>
   <si>
     <t>e SE_z</t>
   </si>
   <si>
-    <t>e'_z</t>
-  </si>
-  <si>
-    <t>e' SE_z</t>
-  </si>
-  <si>
     <t>SES index 1: Parental education and occupation at 18 months</t>
   </si>
   <si>
@@ -370,12 +322,6 @@
     <t>CITO-elementary test (national test of educational achievement: composite)</t>
   </si>
   <si>
-    <t>broad factor/compsite</t>
-  </si>
-  <si>
-    <t>achievement/Gc</t>
-  </si>
-  <si>
     <t>Jacobson (unpublished)</t>
   </si>
   <si>
@@ -481,7 +427,61 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Zcheck_</t>
+    <t>N Pairs</t>
+  </si>
+  <si>
+    <t>broad vs composite</t>
+  </si>
+  <si>
+    <t>achievement vs Gc</t>
+  </si>
+  <si>
+    <t>Age Yrs</t>
+  </si>
+  <si>
+    <t>a SE</t>
+  </si>
+  <si>
+    <t>a SE z</t>
+  </si>
+  <si>
+    <t>Zcheck</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a1 SE</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c1 SE</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e1 SE</t>
+  </si>
+  <si>
+    <t>a1_z</t>
+  </si>
+  <si>
+    <t>a1 SE_z</t>
+  </si>
+  <si>
+    <t>c1_z</t>
+  </si>
+  <si>
+    <t>c1 SE_z</t>
+  </si>
+  <si>
+    <t>e1_z</t>
+  </si>
+  <si>
+    <t>e1 SE_z</t>
   </si>
 </sst>
 </file>
@@ -1119,10 +1119,10 @@
   <dimension ref="A1:AU50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="AT29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AT51" sqref="AT51"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1163,55 +1163,55 @@
   <sheetData>
     <row r="1" spans="1:47" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>4</v>
@@ -1223,85 +1223,85 @@
         <v>6</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="AD1" s="1" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:47" s="6" customFormat="1">
@@ -1309,10 +1309,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -1327,13 +1327,13 @@
         <v>125</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K2" s="7">
         <v>1</v>
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P2" s="6">
         <v>1</v>
@@ -1450,10 +1450,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -1468,13 +1468,13 @@
         <v>125</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K3" s="7">
         <v>1</v>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P3" s="6">
         <v>1</v>
@@ -1591,10 +1591,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
@@ -1609,19 +1609,19 @@
         <v>125</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K4" s="7">
         <v>1</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="M4" s="7">
         <v>0</v>
@@ -1630,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P4" s="6">
         <v>1</v>
@@ -1732,10 +1732,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -1750,19 +1750,19 @@
         <v>125</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K5" s="7">
         <v>1</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M5" s="7">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>1</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P5" s="6">
         <v>1</v>
@@ -1873,10 +1873,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -1891,19 +1891,19 @@
         <v>125</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K6" s="7">
         <v>1</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M6" s="7">
         <v>0</v>
@@ -1912,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P6" s="6">
         <v>1</v>
@@ -2014,10 +2014,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -2032,19 +2032,19 @@
         <v>125</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K7" s="7">
         <v>1</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="M7" s="7">
         <v>0</v>
@@ -2053,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P7" s="6">
         <v>1</v>
@@ -2155,10 +2155,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -2173,19 +2173,19 @@
         <v>106.33333330000001</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K8" s="7">
         <v>1</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="M8" s="6">
         <v>0</v>
@@ -2194,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P8" s="6">
         <v>1</v>
@@ -2296,10 +2296,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6">
         <v>2</v>
@@ -2314,19 +2314,19 @@
         <v>106.33333330000001</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K9" s="7">
         <v>1</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M9" s="6">
         <v>1</v>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P9" s="6">
         <v>1</v>
@@ -2437,10 +2437,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
@@ -2455,20 +2455,20 @@
         <v>106.33333330000001</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="7">
+        <v>1</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="7">
-        <v>1</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="M10" s="6">
         <v>0</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P10" s="6">
         <v>1</v>
@@ -2578,10 +2578,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6">
         <v>3</v>
@@ -2596,19 +2596,19 @@
         <v>419.5</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="M11" s="6">
         <v>1</v>
@@ -2617,7 +2617,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P11" s="6">
         <v>1</v>
@@ -2719,10 +2719,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D12" s="6">
         <v>3</v>
@@ -2737,19 +2737,19 @@
         <v>419.5</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="M12" s="6">
         <v>1</v>
@@ -2758,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P12" s="6">
         <v>1</v>
@@ -2860,10 +2860,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D13" s="6">
         <v>4</v>
@@ -2878,19 +2878,19 @@
         <v>851</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K13" s="7">
         <v>1</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M13" s="6">
         <v>1</v>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P13" s="6">
         <v>1</v>
@@ -3001,10 +3001,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D14" s="6">
         <v>5</v>
@@ -3019,19 +3019,19 @@
         <v>1601.5</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="M14" s="6">
         <v>1</v>
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P14" s="6">
         <v>1</v>
@@ -3142,10 +3142,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D15" s="6">
         <v>5</v>
@@ -3160,19 +3160,19 @@
         <v>173.5</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="M15" s="6">
         <v>0</v>
@@ -3181,7 +3181,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P15" s="6">
         <v>1</v>
@@ -3283,10 +3283,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D16" s="6">
         <v>6</v>
@@ -3301,19 +3301,19 @@
         <v>544.75</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K16" s="7">
         <v>1</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M16" s="6">
         <v>1</v>
@@ -3322,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P16" s="6">
         <v>0</v>
@@ -3424,10 +3424,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6">
         <v>6</v>
@@ -3442,19 +3442,19 @@
         <v>544.75</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K17" s="7">
         <v>1</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M17" s="6">
         <v>1</v>
@@ -3463,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P17" s="6">
         <v>0</v>
@@ -3565,10 +3565,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D18" s="6">
         <v>6</v>
@@ -3583,19 +3583,19 @@
         <v>544.75</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K18" s="7">
         <v>1</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M18" s="6">
         <v>1</v>
@@ -3604,7 +3604,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P18" s="6">
         <v>0</v>
@@ -3706,10 +3706,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D19" s="6">
         <v>6</v>
@@ -3724,19 +3724,19 @@
         <v>544.75</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="K19" s="7">
         <v>1</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M19" s="6">
         <v>1</v>
@@ -3745,7 +3745,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P19" s="6">
         <v>0</v>
@@ -3847,10 +3847,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D20" s="6">
         <v>6</v>
@@ -3865,19 +3865,19 @@
         <v>544.75</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="K20" s="6">
         <v>0</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M20" s="6">
         <v>1</v>
@@ -3886,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P20" s="6">
         <v>0</v>
@@ -3988,10 +3988,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D21" s="6">
         <v>6</v>
@@ -4006,19 +4006,19 @@
         <v>544.75</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K21" s="7">
         <v>1</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M21" s="6">
         <v>1</v>
@@ -4027,7 +4027,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P21" s="6">
         <v>0</v>
@@ -4129,10 +4129,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D22" s="6">
         <v>6</v>
@@ -4147,19 +4147,19 @@
         <v>544.75</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="K22" s="7">
         <v>1</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M22" s="6">
         <v>1</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P22" s="6">
         <v>0</v>
@@ -4270,10 +4270,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D23" s="6">
         <v>6</v>
@@ -4288,19 +4288,19 @@
         <v>544.75</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K23" s="7">
         <v>1</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M23" s="6">
         <v>1</v>
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P23" s="6">
         <v>0</v>
@@ -4411,10 +4411,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D24" s="6">
         <v>6</v>
@@ -4429,19 +4429,19 @@
         <v>544.75</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="K24" s="6">
         <v>0</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M24" s="6">
         <v>1</v>
@@ -4450,7 +4450,7 @@
         <v>0</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P24" s="6">
         <v>0</v>
@@ -4552,10 +4552,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D25" s="6">
         <v>6</v>
@@ -4570,19 +4570,19 @@
         <v>544.75</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="K25" s="7">
         <v>1</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M25" s="6">
         <v>1</v>
@@ -4591,7 +4591,7 @@
         <v>0</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P25" s="6">
         <v>0</v>
@@ -4693,10 +4693,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D26" s="6">
         <v>6</v>
@@ -4711,19 +4711,19 @@
         <v>544.75</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="K26" s="6">
         <v>0</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M26" s="6">
         <v>1</v>
@@ -4732,7 +4732,7 @@
         <v>0</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P26" s="6">
         <v>0</v>
@@ -4834,10 +4834,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D27" s="6">
         <v>6</v>
@@ -4852,19 +4852,19 @@
         <v>544.75</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="K27" s="7">
         <v>1</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M27" s="6">
         <v>1</v>
@@ -4873,7 +4873,7 @@
         <v>0</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P27" s="6">
         <v>0</v>
@@ -4975,10 +4975,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D28" s="6">
         <v>6</v>
@@ -4993,19 +4993,19 @@
         <v>544.75</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K28" s="7">
         <v>1</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M28" s="6">
         <v>1</v>
@@ -5014,7 +5014,7 @@
         <v>0</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P28" s="6">
         <v>0</v>
@@ -5116,10 +5116,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D29" s="6">
         <v>6</v>
@@ -5134,19 +5134,19 @@
         <v>544.75</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="K29" s="7">
         <v>1</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M29" s="6">
         <v>1</v>
@@ -5155,7 +5155,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P29" s="6">
         <v>0</v>
@@ -5257,10 +5257,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D30" s="6">
         <v>6</v>
@@ -5275,19 +5275,19 @@
         <v>544.75</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K30" s="7">
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M30" s="6">
         <v>1</v>
@@ -5296,7 +5296,7 @@
         <v>0</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P30" s="6">
         <v>0</v>
@@ -5398,10 +5398,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D31" s="6">
         <v>6</v>
@@ -5416,19 +5416,19 @@
         <v>544.75</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="K31" s="6">
         <v>0</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M31" s="6">
         <v>1</v>
@@ -5437,7 +5437,7 @@
         <v>0</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="P31" s="6">
         <v>0</v>
@@ -5539,10 +5539,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D32" s="6">
         <v>7</v>
@@ -5557,19 +5557,19 @@
         <v>466</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K32" s="7">
         <v>1</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="M32" s="6">
         <v>0</v>
@@ -5578,7 +5578,7 @@
         <v>1</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P32" s="6">
         <v>1</v>
@@ -5680,10 +5680,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D33" s="6">
         <v>8</v>
@@ -5698,19 +5698,19 @@
         <v>1176</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K33" s="6">
         <v>0</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M33" s="6">
         <v>1</v>
@@ -5719,7 +5719,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="P33" s="6">
         <v>0</v>
@@ -5821,10 +5821,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D34" s="6">
         <v>9</v>
@@ -5839,19 +5839,19 @@
         <v>107.5</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="K34" s="7">
         <v>1</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M34" s="6">
         <v>0</v>
@@ -5860,7 +5860,7 @@
         <v>1</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="P34" s="6">
         <v>0</v>
@@ -5962,10 +5962,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D35" s="6">
         <v>9</v>
@@ -5980,19 +5980,19 @@
         <v>107.5</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="K35" s="7">
         <v>1</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="M35" s="6">
         <v>0</v>
@@ -6001,7 +6001,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="P35" s="6">
         <v>0</v>
@@ -6103,10 +6103,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D36" s="6">
         <v>10</v>
@@ -6121,28 +6121,28 @@
         <v>954.5</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K36" s="6">
         <v>0</v>
       </c>
       <c r="L36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" s="6">
+        <v>0</v>
+      </c>
+      <c r="N36" s="6">
+        <v>1</v>
+      </c>
+      <c r="O36" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="M36" s="6">
-        <v>0</v>
-      </c>
-      <c r="N36" s="6">
-        <v>1</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="P36" s="6">
         <v>1</v>
@@ -6244,10 +6244,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D37" s="6">
         <v>10</v>
@@ -6262,28 +6262,28 @@
         <v>623</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K37" s="6">
         <v>0</v>
       </c>
       <c r="L37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M37" s="6">
+        <v>0</v>
+      </c>
+      <c r="N37" s="6">
+        <v>1</v>
+      </c>
+      <c r="O37" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="M37" s="6">
-        <v>0</v>
-      </c>
-      <c r="N37" s="6">
-        <v>1</v>
-      </c>
-      <c r="O37" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="P37" s="6">
         <v>1</v>
@@ -6385,10 +6385,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D38" s="6">
         <v>11</v>
@@ -6403,19 +6403,19 @@
         <v>2494</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K38" s="7">
         <v>1</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="M38" s="6">
         <v>1</v>
@@ -6424,7 +6424,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P38" s="6">
         <v>1</v>
@@ -6526,10 +6526,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D39" s="6">
         <v>12</v>
@@ -6544,19 +6544,19 @@
         <v>3132</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K39" s="6">
         <v>0</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="M39" s="6">
         <v>1</v>
@@ -6565,7 +6565,7 @@
         <v>1</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P39" s="6">
         <v>0</v>
@@ -6667,10 +6667,10 @@
         <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D40" s="6">
         <v>13</v>
@@ -6685,19 +6685,19 @@
         <v>542</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K40" s="6">
         <v>0</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="M40" s="6">
         <v>1</v>
@@ -6706,7 +6706,7 @@
         <v>0</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="P40" s="6">
         <v>0</v>
@@ -6808,10 +6808,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D41" s="6">
         <v>14</v>
@@ -6826,19 +6826,19 @@
         <v>89</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K41" s="6">
         <v>0</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M41" s="6">
         <v>1</v>
@@ -6847,7 +6847,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P41" s="6">
         <v>0</v>
@@ -6949,10 +6949,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D42" s="6">
         <v>15</v>
@@ -6967,19 +6967,19 @@
         <v>95.5</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K42" s="6">
         <v>0</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M42" s="6">
         <v>1</v>
@@ -6988,7 +6988,7 @@
         <v>0</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P42" s="6">
         <v>0</v>
@@ -7090,10 +7090,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D43" s="6">
         <v>16</v>
@@ -7108,19 +7108,19 @@
         <v>64</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K43" s="6">
         <v>0</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M43" s="6">
         <v>1</v>
@@ -7129,7 +7129,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P43" s="6">
         <v>0</v>
@@ -7231,10 +7231,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D44" s="6">
         <v>17</v>
@@ -7249,19 +7249,19 @@
         <v>101.5</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K44" s="6">
         <v>0</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M44" s="6">
         <v>1</v>
@@ -7270,7 +7270,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P44" s="6">
         <v>0</v>
@@ -7372,133 +7372,133 @@
         <v>0</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D45" s="6">
         <v>18</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P45" s="6">
         <v>0</v>
       </c>
       <c r="Q45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="R45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="S45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="U45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="W45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="X45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Y45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Z45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AA45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AB45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AC45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AD45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AE45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AF45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AH45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AI45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AJ45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AK45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AL45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AM45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AN45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AO45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AP45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AQ45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AR45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AS45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AT45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AU45" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:47" s="6" customFormat="1">
@@ -7506,139 +7506,139 @@
         <v>0</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D46" s="6">
         <v>19</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P46" s="6">
         <v>1</v>
       </c>
       <c r="Q46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="S46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="U46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="V46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="W46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="X46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Z46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AA46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AB46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AC46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AD46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AE46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AF46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AH46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AI46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AJ46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AK46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AL46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AM46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AN46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AO46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AP46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AQ46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AR46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AS46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AT46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AU46" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:47" s="6" customFormat="1">
@@ -7646,10 +7646,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D47" s="6">
         <v>20</v>
@@ -7664,28 +7664,28 @@
         <v>1307</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="P47" s="6">
         <v>0</v>
@@ -7694,91 +7694,91 @@
         <v>8</v>
       </c>
       <c r="R47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="S47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="T47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="U47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="V47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="W47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="X47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Y47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Z47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AA47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AB47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AC47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AD47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AE47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AF47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AH47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AI47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AJ47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AK47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AL47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AM47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AN47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AO47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AP47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AQ47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AR47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AS47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AT47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AU47" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:47" s="6" customFormat="1">
@@ -7786,10 +7786,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D48" s="6">
         <v>20</v>
@@ -7804,28 +7804,28 @@
         <v>1235</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="P48" s="6">
         <v>0</v>
@@ -7834,91 +7834,91 @@
         <v>10</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="S48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="T48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="U48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="V48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="W48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="X48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Y48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Z48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AA48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AB48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AC48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AD48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AE48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AF48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AH48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AI48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AJ48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AK48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AL48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AM48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AN48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AO48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AP48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AQ48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AR48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AS48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AT48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AU48" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:47" s="6" customFormat="1">
@@ -7926,10 +7926,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D49" s="6">
         <v>20</v>
@@ -7944,28 +7944,28 @@
         <v>1076</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="P49" s="6">
         <v>0</v>
@@ -7974,91 +7974,91 @@
         <v>12</v>
       </c>
       <c r="R49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="U49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="V49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="X49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Y49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Z49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AA49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AB49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AC49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AD49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AE49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AF49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AH49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AI49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AJ49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AK49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AL49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AM49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AN49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AO49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AP49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AQ49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AR49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AS49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AT49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AU49" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:47" s="6" customFormat="1">
@@ -8066,10 +8066,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D50" s="6">
         <v>20</v>
@@ -8084,28 +8084,28 @@
         <v>930</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="O50" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="P50" s="6">
         <v>0</v>
@@ -8114,91 +8114,91 @@
         <v>14</v>
       </c>
       <c r="R50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="S50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="T50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="U50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="V50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="W50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="X50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Y50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="Z50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AA50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AB50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AC50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AD50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AE50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AF50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AH50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AI50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AJ50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AK50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AL50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AM50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AN50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AO50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AP50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AQ50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AR50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AS50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AT50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="AU50" s="6" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating the summary stats file; use metasem; think about histogram and forest plot options
</commit_message>
<xml_diff>
--- a/inst/extdata/GxSES/data_GxSES.xlsx
+++ b/inst/extdata/GxSES/data_GxSES.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="165">
   <si>
     <t>Bayley</t>
   </si>
@@ -397,15 +397,6 @@
     <t>Figlio, et al. (2017)</t>
   </si>
   <si>
-    <t>10.1016/j.lindif.2017.01.018</t>
-  </si>
-  <si>
-    <t>Schwabe et al. (2017)</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -482,6 +473,42 @@
   </si>
   <si>
     <t>e1 SE_z</t>
+  </si>
+  <si>
+    <t>Eric 2015 Louisville</t>
+  </si>
+  <si>
+    <t>Eric Norway</t>
+  </si>
+  <si>
+    <t>Maternal Education and zip income</t>
+  </si>
+  <si>
+    <t>10.1007/s10519-015-9760-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hollingshead </t>
+  </si>
+  <si>
+    <t>Louisville Twin Study</t>
+  </si>
+  <si>
+    <t>LTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1007/s10519-017-9857-z </t>
+  </si>
+  <si>
+    <t>Norwegian Male conscripts</t>
+  </si>
+  <si>
+    <t>NOR</t>
+  </si>
+  <si>
+    <t>g (Arithmetic, Similarities and Figures)</t>
+  </si>
+  <si>
+    <t>Norway</t>
   </si>
 </sst>
 </file>
@@ -491,7 +518,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +574,21 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Optima Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="BcwwljAdvPTimes"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="AdvTTc999d02f"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="NpvqjbSTIX"/>
     </font>
   </fonts>
   <fills count="2">
@@ -650,7 +692,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -697,6 +739,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1116,32 +1161,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU50"/>
+  <dimension ref="A1:AU53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S31" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="AG35" sqref="AG35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="4"/>
-    <col min="2" max="2" width="33" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="4" customWidth="1"/>
     <col min="6" max="6" width="4.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="34.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="4" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="4" customWidth="1"/>
     <col min="10" max="11" width="19.5" style="4" customWidth="1"/>
     <col min="12" max="12" width="20.83203125" style="4" customWidth="1"/>
     <col min="13" max="13" width="14.33203125" style="4" customWidth="1"/>
     <col min="14" max="14" width="15.1640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20.83203125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="20.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.5" style="4" customWidth="1"/>
     <col min="19" max="19" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -1163,19 +1208,19 @@
   <sheetData>
     <row r="1" spans="1:47" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>54</v>
@@ -1199,10 +1244,10 @@
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>55</v>
@@ -1211,7 +1256,7 @@
         <v>48</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>4</v>
@@ -1223,13 +1268,13 @@
         <v>6</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>7</v>
@@ -1238,10 +1283,10 @@
         <v>10</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>8</v>
@@ -1250,13 +1295,13 @@
         <v>9</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>52</v>
@@ -1271,13 +1316,13 @@
         <v>89</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>90</v>
@@ -1286,10 +1331,10 @@
         <v>91</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>92</v>
@@ -1298,10 +1343,10 @@
         <v>93</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:47" s="6" customFormat="1">
@@ -1309,10 +1354,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -1450,10 +1495,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -1591,10 +1636,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
@@ -1732,10 +1777,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -1873,10 +1918,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -2014,10 +2059,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -2155,10 +2200,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -2296,10 +2341,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D9" s="6">
         <v>2</v>
@@ -2437,10 +2482,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
@@ -2578,10 +2623,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="D11" s="6">
         <v>3</v>
@@ -2719,10 +2764,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="6">
         <v>3</v>
@@ -2860,10 +2905,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="D13" s="6">
         <v>4</v>
@@ -3001,10 +3046,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D14" s="6">
         <v>5</v>
@@ -3142,10 +3187,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D15" s="6">
         <v>5</v>
@@ -3283,10 +3328,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D16" s="6">
         <v>6</v>
@@ -3424,10 +3469,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D17" s="6">
         <v>6</v>
@@ -3565,10 +3610,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D18" s="6">
         <v>6</v>
@@ -3706,10 +3751,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D19" s="6">
         <v>6</v>
@@ -3847,10 +3892,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D20" s="6">
         <v>6</v>
@@ -3988,10 +4033,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D21" s="6">
         <v>6</v>
@@ -4129,10 +4174,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D22" s="6">
         <v>6</v>
@@ -4270,10 +4315,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D23" s="6">
         <v>6</v>
@@ -4411,10 +4456,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D24" s="6">
         <v>6</v>
@@ -4552,10 +4597,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D25" s="6">
         <v>6</v>
@@ -4693,10 +4738,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D26" s="6">
         <v>6</v>
@@ -4834,10 +4879,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D27" s="6">
         <v>6</v>
@@ -4975,10 +5020,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D28" s="6">
         <v>6</v>
@@ -5116,10 +5161,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D29" s="6">
         <v>6</v>
@@ -5257,10 +5302,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D30" s="6">
         <v>6</v>
@@ -5398,10 +5443,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D31" s="6">
         <v>6</v>
@@ -5539,10 +5584,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="D32" s="6">
         <v>7</v>
@@ -5557,7 +5602,7 @@
         <v>466</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>103</v>
@@ -5679,11 +5724,11 @@
       <c r="A33" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="D33" s="6">
         <v>8</v>
@@ -5719,7 +5764,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P33" s="6">
         <v>0</v>
@@ -5821,10 +5866,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="D34" s="6">
         <v>9</v>
@@ -5961,11 +6006,11 @@
       <c r="A35" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="D35" s="6">
         <v>9</v>
@@ -6103,10 +6148,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="D36" s="6">
         <v>10</v>
@@ -6244,10 +6289,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="D37" s="6">
         <v>10</v>
@@ -6262,7 +6307,7 @@
         <v>623</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>102</v>
@@ -6385,10 +6430,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="D38" s="6">
         <v>11</v>
@@ -6526,10 +6571,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="D39" s="6">
         <v>12</v>
@@ -6667,10 +6712,10 @@
         <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="D40" s="6">
         <v>13</v>
@@ -6685,7 +6730,7 @@
         <v>542</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>75</v>
@@ -6808,10 +6853,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D41" s="6">
         <v>14</v>
@@ -6949,10 +6994,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D42" s="6">
         <v>15</v>
@@ -7090,10 +7135,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D43" s="6">
         <v>16</v>
@@ -7231,10 +7276,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D44" s="6">
         <v>17</v>
@@ -7372,133 +7417,139 @@
         <v>0</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="D45" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>136</v>
+        <v>155</v>
+      </c>
+      <c r="K45" s="6">
+        <v>1</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="M45" s="6">
+        <v>0</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="P45" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="R45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="S45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="U45" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="V45" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="W45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="V45" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="W45" s="6">
+        <v>2.2100000000000002E-2</v>
       </c>
       <c r="X45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Y45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Z45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AA45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AB45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AD45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AE45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AF45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AH45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AI45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AJ45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AK45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AL45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AN45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AO45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AP45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AQ45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AR45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AS45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AT45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AU45" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:47" s="6" customFormat="1">
@@ -7506,162 +7557,162 @@
         <v>0</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="D46" s="6">
-        <v>19</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>136</v>
+        <v>20</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1307</v>
+      </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1307</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>136</v>
+        <v>27</v>
+      </c>
+      <c r="K46" s="6">
+        <v>0</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="M46" s="6" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="M46" s="6">
+        <v>0</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="P46" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="6" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>8</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="S46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="U46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="W46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="X46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Z46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AA46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AB46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AD46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AE46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AF46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AH46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AI46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AJ46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AK46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AL46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AN46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AO46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AP46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AQ46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AR46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AS46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AT46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AU46" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:47" s="6" customFormat="1">
       <c r="A47" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="B47" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>132</v>
+      <c r="B47" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="D47" s="6">
         <v>20</v>
       </c>
       <c r="E47" s="6">
-        <v>1307</v>
+        <v>1235</v>
       </c>
       <c r="F47" s="6">
         <v>1</v>
       </c>
       <c r="G47" s="6">
-        <v>1307</v>
+        <v>1235</v>
       </c>
       <c r="H47" s="15" t="s">
         <v>123</v>
@@ -7672,136 +7723,136 @@
       <c r="J47" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K47" s="6" t="s">
-        <v>136</v>
+      <c r="K47" s="6">
+        <v>0</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="M47" s="6">
+        <v>0</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P47" s="6">
         <v>0</v>
       </c>
       <c r="Q47" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="S47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="T47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="U47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="W47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="X47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Y47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Z47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AA47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AB47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AD47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AE47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AF47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AH47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AI47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AJ47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AK47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AL47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AN47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AO47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AP47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AQ47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AR47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AS47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AT47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AU47" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:47" s="6" customFormat="1">
       <c r="A48" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>132</v>
+      <c r="B48" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="D48" s="6">
         <v>20</v>
       </c>
       <c r="E48" s="6">
-        <v>1235</v>
+        <v>1076</v>
       </c>
       <c r="F48" s="6">
         <v>1</v>
       </c>
       <c r="G48" s="6">
-        <v>1235</v>
+        <v>1076</v>
       </c>
       <c r="H48" s="15" t="s">
         <v>123</v>
@@ -7812,136 +7863,136 @@
       <c r="J48" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K48" s="6" t="s">
-        <v>136</v>
+      <c r="K48" s="6">
+        <v>0</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="M48" s="6" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="M48" s="6">
+        <v>0</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P48" s="6">
         <v>0</v>
       </c>
       <c r="Q48" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="S48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="T48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="U48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="W48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="X48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Y48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Z48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AA48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AB48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AD48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AE48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AF48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AH48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AI48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AJ48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AK48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AL48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AN48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AO48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AP48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AQ48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AR48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AS48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AT48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AU48" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:47" s="6" customFormat="1">
       <c r="A49" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>132</v>
+      <c r="B49" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="D49" s="6">
         <v>20</v>
       </c>
       <c r="E49" s="6">
-        <v>1076</v>
+        <v>930</v>
       </c>
       <c r="F49" s="6">
         <v>1</v>
       </c>
       <c r="G49" s="6">
-        <v>1076</v>
+        <v>930</v>
       </c>
       <c r="H49" s="15" t="s">
         <v>123</v>
@@ -7952,257 +8003,368 @@
       <c r="J49" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K49" s="6" t="s">
-        <v>136</v>
+      <c r="K49" s="6">
+        <v>0</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="M49" s="6">
+        <v>0</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P49" s="6">
         <v>0</v>
       </c>
       <c r="Q49" s="8">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="U49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="X49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Y49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Z49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AA49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AB49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AD49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AE49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AF49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AH49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AI49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AJ49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AK49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AL49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AN49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AO49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AP49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AQ49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AR49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AS49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AT49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AU49" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:47" s="6" customFormat="1">
+    <row r="50" spans="1:47">
       <c r="A50" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="6">
+      <c r="B50" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="4">
+        <v>21</v>
+      </c>
+      <c r="E50" s="4">
+        <v>472</v>
+      </c>
+      <c r="F50" s="3">
+        <v>3</v>
+      </c>
+      <c r="G50" s="4">
+        <f>E50/F50</f>
+        <v>157.33333333333334</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="J50" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="K50" s="4">
+        <v>1</v>
+      </c>
+      <c r="L50" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="6">
-        <v>930</v>
-      </c>
-      <c r="F50" s="6">
-        <v>1</v>
-      </c>
-      <c r="G50" s="6">
-        <v>930</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="I50" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J50" s="6" t="s">
+      <c r="M50" s="6">
+        <v>0</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:47">
+      <c r="A51" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="4">
+        <v>21</v>
+      </c>
+      <c r="E51" s="4">
+        <v>472</v>
+      </c>
+      <c r="F51" s="3">
+        <v>3</v>
+      </c>
+      <c r="G51" s="4">
+        <f t="shared" ref="G51:G52" si="0">E51/F51</f>
+        <v>157.33333333333334</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="J51" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="K51" s="4">
+        <v>1</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M51" s="6">
+        <v>0</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:47">
+      <c r="A52" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D52" s="4">
+        <v>21</v>
+      </c>
+      <c r="E52" s="4">
+        <v>472</v>
+      </c>
+      <c r="F52" s="3">
+        <v>3</v>
+      </c>
+      <c r="G52" s="4">
+        <f t="shared" si="0"/>
+        <v>157.33333333333334</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="J52" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="K52" s="4">
+        <v>1</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" s="6">
+        <v>1</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:47">
+      <c r="A53" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D53" s="4">
+        <v>22</v>
+      </c>
+      <c r="E53" s="19">
+        <v>1706</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1706</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J53" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="L50" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="M50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="N50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="O50" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="P50" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="8">
-        <v>14</v>
-      </c>
-      <c r="R50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="S50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="T50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="U50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="V50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="W50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="X50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AE50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AH50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AJ50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AK50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AM50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AN50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AO50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AP50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AQ50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AR50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AS50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AT50" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AU50" s="6" t="s">
-        <v>136</v>
+      <c r="K53" s="4">
+        <v>0</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="N53" s="4">
+        <v>1</v>
+      </c>
+      <c r="O53" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P53" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="5">
+        <v>20</v>
+      </c>
+      <c r="T53" s="20">
+        <v>0.89</v>
+      </c>
+      <c r="U53" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="V53" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="W53" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="X53" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="Y53" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="Z53" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="AA53" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="AJ53" s="20">
+        <v>0.89</v>
+      </c>
+      <c r="AK53" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="AL53" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AM53" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="AN53" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="AO53" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="AP53" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="AQ53" s="4">
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:AY46">
+  <sortState ref="C2:AY45">
     <sortCondition ref="D1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>